<commit_message>
Slightly improved heuristic and added randomness
</commit_message>
<xml_diff>
--- a/results/AI vs random.xlsx
+++ b/results/AI vs random.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="18">
   <si>
     <t>Tree depth</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>AveragePieces</t>
+  </si>
+  <si>
+    <t>(player_pieces_count - AI_pieces_count) + (possible_player_moves - possible_AI_moves)</t>
+  </si>
+  <si>
+    <t>( (player_pieces_count+possible_player_moves) - (AI_pieces_count+possible_AI_moves)</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>( (player_pieces_count + possible_player_flips) - (AI_pieces_count+possible_AI_flips))</t>
   </si>
 </sst>
 </file>
@@ -386,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F99"/>
+  <dimension ref="A2:F240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="D241" sqref="D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +435,30 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
@@ -716,24 +752,17 @@
         <v>35.07692307692308</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>10</v>
-      </c>
-      <c r="E26">
-        <v>50</v>
-      </c>
-      <c r="F26" t="s">
-        <v>8</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <f>STDEV(D11:D23)</f>
+        <v>11.574729326181197</v>
+      </c>
+      <c r="E25">
+        <f>STDEV(E11:E23)</f>
+        <v>7.7616744162319566</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -767,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -787,10 +816,10 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E29">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -807,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E30">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -827,10 +856,10 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E31">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -847,10 +876,10 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -867,10 +896,10 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -887,10 +916,10 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E34">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -907,10 +936,10 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
@@ -927,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -947,10 +976,10 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E37">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
@@ -967,10 +996,10 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E38">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
@@ -987,10 +1016,10 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
@@ -1007,66 +1036,59 @@
         <v>1</v>
       </c>
       <c r="D40">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>51</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
         <v>16</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>22</v>
       </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>13</v>
       </c>
-      <c r="D41">
-        <f>AVERAGE(D26:D40)</f>
+      <c r="D42">
+        <f>AVERAGE(D27:D41)</f>
         <v>16.399999999999999</v>
       </c>
-      <c r="E41">
-        <f>AVERAGE(E26:E40)</f>
+      <c r="E42">
+        <f>AVERAGE(E27:E41)</f>
         <v>38.266666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>3</v>
-      </c>
-      <c r="B43">
-        <v>20</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>16</v>
       </c>
       <c r="D43">
-        <v>33</v>
+        <f>STDEV(D27:D41)</f>
+        <v>10.411532067856296</v>
       </c>
       <c r="E43">
-        <v>31</v>
-      </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44">
-        <v>20</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>15</v>
-      </c>
-      <c r="E44">
-        <v>49</v>
-      </c>
-      <c r="F44" t="s">
-        <v>8</v>
+        <f>STDEV(E27:E41)</f>
+        <v>13.624907164384471</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,7 +1105,7 @@
         <v>33</v>
       </c>
       <c r="E45">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F45" t="s">
         <v>7</v>
@@ -1100,10 +1122,10 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E46">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F46" t="s">
         <v>8</v>
@@ -1120,10 +1142,10 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E47">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F47" t="s">
         <v>7</v>
@@ -1140,13 +1162,13 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49">
+        <v>24</v>
+      </c>
+      <c r="F49" t="s">
         <v>7</v>
-      </c>
-      <c r="E49">
-        <v>45</v>
-      </c>
-      <c r="F49" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1180,13 +1202,13 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1200,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F51" t="s">
         <v>8</v>
@@ -1220,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
         <v>8</v>
@@ -1240,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E53">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
@@ -1260,10 +1282,10 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E54">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F54" t="s">
         <v>8</v>
@@ -1280,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E55">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F55" t="s">
         <v>8</v>
@@ -1300,10 +1322,10 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E56">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
@@ -1320,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
         <v>8</v>
@@ -1340,10 +1362,10 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E58">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F58" t="s">
         <v>8</v>
@@ -1360,86 +1382,79 @@
         <v>1</v>
       </c>
       <c r="D59">
+        <v>25</v>
+      </c>
+      <c r="E59">
+        <v>39</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>28</v>
+      </c>
+      <c r="E60">
+        <v>36</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
         <v>52</v>
       </c>
-      <c r="E59">
+      <c r="E61">
         <v>12</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>13</v>
       </c>
-      <c r="D60">
-        <f>AVERAGE(D43:D59)</f>
+      <c r="D62">
+        <f>AVERAGE(D45:D61)</f>
         <v>21.117647058823529</v>
       </c>
-      <c r="E60">
-        <f>AVERAGE(E43:E59)</f>
+      <c r="E62">
+        <f>AVERAGE(E45:E61)</f>
         <v>32.764705882352942</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>4</v>
-      </c>
-      <c r="B62">
-        <v>10</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>8</v>
-      </c>
-      <c r="E62">
-        <v>55</v>
-      </c>
-      <c r="F62" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>4</v>
-      </c>
-      <c r="B63">
-        <v>10</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
+      <c r="C63" t="s">
+        <v>16</v>
       </c>
       <c r="D63">
-        <v>14</v>
+        <f>STDEV(D45:D61)</f>
+        <v>15.003676020150763</v>
       </c>
       <c r="E63">
-        <v>50</v>
-      </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>4</v>
-      </c>
-      <c r="B64">
-        <v>10</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64">
-        <v>20</v>
-      </c>
-      <c r="E64">
-        <v>44</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
+        <f>STDEV(E45:E61)</f>
+        <v>13.530194990117041</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E65">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
@@ -1473,10 +1488,10 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E66">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
@@ -1493,10 +1508,10 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E67">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F67" t="s">
         <v>8</v>
@@ -1513,10 +1528,10 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E68">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
@@ -1533,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E69">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F69" t="s">
         <v>8</v>
@@ -1553,10 +1568,10 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E70">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F70" t="s">
         <v>8</v>
@@ -1573,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E71">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
         <v>8</v>
@@ -1593,10 +1608,10 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E72">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
@@ -1613,10 +1628,10 @@
         <v>1</v>
       </c>
       <c r="D73">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E73">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F73" t="s">
         <v>8</v>
@@ -1633,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E74">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F74" t="s">
         <v>8</v>
@@ -1653,10 +1668,10 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F75" t="s">
         <v>8</v>
@@ -1673,10 +1688,10 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E76">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F76" t="s">
         <v>8</v>
@@ -1693,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="D77">
+        <v>16</v>
+      </c>
+      <c r="E77">
         <v>38</v>
       </c>
-      <c r="E77">
-        <v>24</v>
-      </c>
       <c r="F77" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1713,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E78">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F78" t="s">
         <v>8</v>
@@ -1733,10 +1748,10 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E79">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
@@ -1753,13 +1768,13 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E80">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,86 +1788,99 @@
         <v>1</v>
       </c>
       <c r="D81">
+        <v>16</v>
+      </c>
+      <c r="E81">
+        <v>47</v>
+      </c>
+      <c r="F81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>24</v>
+      </c>
+      <c r="E82">
+        <v>40</v>
+      </c>
+      <c r="F82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>4</v>
+      </c>
+      <c r="B83">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>13</v>
+      </c>
+      <c r="E83">
+        <v>44</v>
+      </c>
+      <c r="F83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
         <v>14</v>
       </c>
-      <c r="E81">
+      <c r="E84">
         <v>50</v>
       </c>
-      <c r="F81" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
         <v>13</v>
       </c>
-      <c r="D82">
-        <f>AVERAGE(D62:D79)</f>
+      <c r="D85">
+        <f>AVERAGE(D65:D82)</f>
         <v>17.888888888888889</v>
       </c>
-      <c r="E82">
-        <f>AVERAGE(E62:E79)</f>
+      <c r="E85">
+        <f>AVERAGE(E65:E82)</f>
         <v>44.055555555555557</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>5</v>
-      </c>
-      <c r="B85">
-        <v>5</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>28</v>
-      </c>
-      <c r="E85">
-        <v>36</v>
-      </c>
-      <c r="F85" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>5</v>
-      </c>
-      <c r="B86">
-        <v>5</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
+      <c r="C86" t="s">
+        <v>16</v>
       </c>
       <c r="D86">
-        <v>24</v>
+        <f>STDEV(D65:D84)</f>
+        <v>9.8326791337543611</v>
       </c>
       <c r="E86">
-        <v>40</v>
-      </c>
-      <c r="F86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>5</v>
-      </c>
-      <c r="B87">
-        <v>5</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <v>35</v>
-      </c>
-      <c r="F87" t="s">
-        <v>8</v>
+        <f>STDEV(E65:E84)</f>
+        <v>8.6710346617496175</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,13 +1894,13 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E88">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F88" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -1886,10 +1914,10 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E89">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F89" t="s">
         <v>8</v>
@@ -1906,10 +1934,10 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F90" t="s">
         <v>8</v>
@@ -1926,13 +1954,13 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E91">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -1946,13 +1974,13 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E92">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,13 +1994,13 @@
         <v>1</v>
       </c>
       <c r="D93">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E93">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F93" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,10 +2014,10 @@
         <v>1</v>
       </c>
       <c r="D94">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E94">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F94" t="s">
         <v>8</v>
@@ -2006,13 +2034,13 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E95">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F95" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,13 +2054,13 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E96">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="F96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2046,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="D97">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E97">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
@@ -2066,26 +2094,2392 @@
         <v>1</v>
       </c>
       <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>6</v>
+      </c>
+      <c r="E99">
+        <v>56</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>28</v>
+      </c>
+      <c r="E100">
+        <v>36</v>
+      </c>
+      <c r="F100" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
         <v>29</v>
       </c>
-      <c r="E98">
+      <c r="E101">
         <v>35</v>
       </c>
-      <c r="F98" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
+      <c r="F101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
         <v>13</v>
       </c>
-      <c r="D99">
-        <f>AVERAGE(D85:D98)</f>
+      <c r="D102">
+        <f>AVERAGE(D88:D101)</f>
         <v>22</v>
       </c>
-      <c r="E99">
-        <f>AVERAGE(E85:E98)</f>
+      <c r="E102">
+        <f>AVERAGE(E88:E101)</f>
         <v>36.857142857142854</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103">
+        <f>STDEV(D88:D101)</f>
+        <v>12.949606468627055</v>
+      </c>
+      <c r="E103">
+        <f>STDEV(E88:E101)</f>
+        <v>7.2733141621339952</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>3</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>15</v>
+      </c>
+      <c r="E105">
+        <v>49</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <v>27</v>
+      </c>
+      <c r="E106">
+        <v>37</v>
+      </c>
+      <c r="F106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>36</v>
+      </c>
+      <c r="F107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>3</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>29</v>
+      </c>
+      <c r="E108">
+        <v>35</v>
+      </c>
+      <c r="F108" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109">
+        <v>10</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>39</v>
+      </c>
+      <c r="F109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <v>10</v>
+      </c>
+      <c r="E110">
+        <v>53</v>
+      </c>
+      <c r="F110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>14</v>
+      </c>
+      <c r="E111">
+        <v>50</v>
+      </c>
+      <c r="F111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <v>10</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>32</v>
+      </c>
+      <c r="E112">
+        <v>29</v>
+      </c>
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>3</v>
+      </c>
+      <c r="B113">
+        <v>10</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>18</v>
+      </c>
+      <c r="E113">
+        <v>45</v>
+      </c>
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>3</v>
+      </c>
+      <c r="B114">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114">
+        <v>28</v>
+      </c>
+      <c r="E114">
+        <v>35</v>
+      </c>
+      <c r="F114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115">
+        <v>11</v>
+      </c>
+      <c r="E115">
+        <v>52</v>
+      </c>
+      <c r="F115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <v>13</v>
+      </c>
+      <c r="E116">
+        <v>51</v>
+      </c>
+      <c r="F116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>3</v>
+      </c>
+      <c r="B117">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>9</v>
+      </c>
+      <c r="E117">
+        <v>54</v>
+      </c>
+      <c r="F117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>21</v>
+      </c>
+      <c r="E118">
+        <v>43</v>
+      </c>
+      <c r="F118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>10</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119">
+        <v>20</v>
+      </c>
+      <c r="E119">
+        <v>44</v>
+      </c>
+      <c r="F119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>7</v>
+      </c>
+      <c r="E120">
+        <v>34</v>
+      </c>
+      <c r="F120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121">
+        <f>AVERAGE(D105:D120)</f>
+        <v>16.1875</v>
+      </c>
+      <c r="E121">
+        <f>AVERAGE(E105:E120)</f>
+        <v>42.875</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122">
+        <f>STDEV(D105:D120)</f>
+        <v>9.3681641744794373</v>
+      </c>
+      <c r="E122">
+        <f>STDEV(E105:E120)</f>
+        <v>8.0072883466668454</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>10</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+      <c r="D124">
+        <v>23</v>
+      </c>
+      <c r="E124">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>4</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>11</v>
+      </c>
+      <c r="E125">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>4</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>18</v>
+      </c>
+      <c r="E126">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>4</v>
+      </c>
+      <c r="B127">
+        <v>10</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>47</v>
+      </c>
+      <c r="E127">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>17</v>
+      </c>
+      <c r="E128">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>4</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>7</v>
+      </c>
+      <c r="E129">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>4</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130">
+        <v>30</v>
+      </c>
+      <c r="E130">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>4</v>
+      </c>
+      <c r="B131">
+        <v>10</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131">
+        <v>28</v>
+      </c>
+      <c r="E131">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>10</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <v>24</v>
+      </c>
+      <c r="E132">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133">
+        <v>11</v>
+      </c>
+      <c r="E133">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>4</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+      <c r="D134">
+        <v>15</v>
+      </c>
+      <c r="E134">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>4</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>19</v>
+      </c>
+      <c r="E135">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>4</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>18</v>
+      </c>
+      <c r="E136">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>4</v>
+      </c>
+      <c r="B137">
+        <v>10</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <v>36</v>
+      </c>
+      <c r="E137">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>13</v>
+      </c>
+      <c r="D138">
+        <f>AVERAGE(D124:D137)</f>
+        <v>21.714285714285715</v>
+      </c>
+      <c r="E138">
+        <f>AVERAGE(E124:E137)</f>
+        <v>39.571428571428569</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139">
+        <f>STDEV(D124:D137)</f>
+        <v>10.766247624501673</v>
+      </c>
+      <c r="E139">
+        <f>STDEV(E124:E137)</f>
+        <v>9.7799975280340306</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>4</v>
+      </c>
+      <c r="B141">
+        <v>10</v>
+      </c>
+      <c r="C141">
+        <v>3</v>
+      </c>
+      <c r="D141">
+        <v>9</v>
+      </c>
+      <c r="E141">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>4</v>
+      </c>
+      <c r="B142">
+        <v>10</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>14</v>
+      </c>
+      <c r="E142">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>4</v>
+      </c>
+      <c r="B143">
+        <v>10</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143">
+        <v>24</v>
+      </c>
+      <c r="E143">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>4</v>
+      </c>
+      <c r="B144">
+        <v>10</v>
+      </c>
+      <c r="C144">
+        <v>3</v>
+      </c>
+      <c r="D144">
+        <v>36</v>
+      </c>
+      <c r="E144">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>4</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+      <c r="D145">
+        <v>14</v>
+      </c>
+      <c r="E145">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>4</v>
+      </c>
+      <c r="B146">
+        <v>10</v>
+      </c>
+      <c r="C146">
+        <v>3</v>
+      </c>
+      <c r="D146">
+        <v>10</v>
+      </c>
+      <c r="E146">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>4</v>
+      </c>
+      <c r="B147">
+        <v>10</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147">
+        <v>44</v>
+      </c>
+      <c r="E147">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>4</v>
+      </c>
+      <c r="B148">
+        <v>10</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>17</v>
+      </c>
+      <c r="E148">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>4</v>
+      </c>
+      <c r="B149">
+        <v>10</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149">
+        <v>43</v>
+      </c>
+      <c r="E149">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>4</v>
+      </c>
+      <c r="B150">
+        <v>10</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150">
+        <v>12</v>
+      </c>
+      <c r="E150">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>4</v>
+      </c>
+      <c r="B151">
+        <v>10</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+      <c r="D151">
+        <v>6</v>
+      </c>
+      <c r="E151">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>4</v>
+      </c>
+      <c r="B152">
+        <v>10</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+      <c r="D152">
+        <v>14</v>
+      </c>
+      <c r="E152">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="B153">
+        <v>10</v>
+      </c>
+      <c r="C153">
+        <v>3</v>
+      </c>
+      <c r="D153">
+        <v>21</v>
+      </c>
+      <c r="E153">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="B154">
+        <v>10</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154">
+        <v>6</v>
+      </c>
+      <c r="E154">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>4</v>
+      </c>
+      <c r="B155">
+        <v>10</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
+      <c r="D155">
+        <v>26</v>
+      </c>
+      <c r="E155">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156">
+        <f>AVERAGE(D141:D155)</f>
+        <v>19.733333333333334</v>
+      </c>
+      <c r="E156">
+        <f>AVERAGE(E141:E155)</f>
+        <v>40.533333333333331</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>16</v>
+      </c>
+      <c r="D157">
+        <f>STDEV(D141:D155)</f>
+        <v>12.555401038521042</v>
+      </c>
+      <c r="E157">
+        <f>STDEV(E141:E155)</f>
+        <v>11.115411866070504</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>2</v>
+      </c>
+      <c r="B160">
+        <v>10</v>
+      </c>
+      <c r="C160">
+        <v>4</v>
+      </c>
+      <c r="D160">
+        <v>4</v>
+      </c>
+      <c r="E160">
+        <v>12</v>
+      </c>
+      <c r="F160" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2</v>
+      </c>
+      <c r="B161">
+        <v>10</v>
+      </c>
+      <c r="C161">
+        <v>4</v>
+      </c>
+      <c r="D161">
+        <v>23</v>
+      </c>
+      <c r="E161">
+        <v>41</v>
+      </c>
+      <c r="F161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>2</v>
+      </c>
+      <c r="B162">
+        <v>10</v>
+      </c>
+      <c r="C162">
+        <v>4</v>
+      </c>
+      <c r="D162">
+        <v>13</v>
+      </c>
+      <c r="E162">
+        <v>37</v>
+      </c>
+      <c r="F162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2</v>
+      </c>
+      <c r="B163">
+        <v>10</v>
+      </c>
+      <c r="C163">
+        <v>4</v>
+      </c>
+      <c r="D163">
+        <v>29</v>
+      </c>
+      <c r="E163">
+        <v>33</v>
+      </c>
+      <c r="F163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2</v>
+      </c>
+      <c r="B164">
+        <v>10</v>
+      </c>
+      <c r="C164">
+        <v>4</v>
+      </c>
+      <c r="D164">
+        <v>32</v>
+      </c>
+      <c r="E164">
+        <v>30</v>
+      </c>
+      <c r="F164" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>2</v>
+      </c>
+      <c r="B165">
+        <v>10</v>
+      </c>
+      <c r="C165">
+        <v>4</v>
+      </c>
+      <c r="D165">
+        <v>18</v>
+      </c>
+      <c r="E165">
+        <v>34</v>
+      </c>
+      <c r="F165" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>2</v>
+      </c>
+      <c r="B166">
+        <v>10</v>
+      </c>
+      <c r="C166">
+        <v>4</v>
+      </c>
+      <c r="D166">
+        <v>31</v>
+      </c>
+      <c r="E166">
+        <v>33</v>
+      </c>
+      <c r="F166" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2</v>
+      </c>
+      <c r="B167">
+        <v>10</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167">
+        <v>24</v>
+      </c>
+      <c r="E167">
+        <v>39</v>
+      </c>
+      <c r="F167" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>2</v>
+      </c>
+      <c r="B168">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <v>4</v>
+      </c>
+      <c r="D168">
+        <v>26</v>
+      </c>
+      <c r="E168">
+        <v>38</v>
+      </c>
+      <c r="F168" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2</v>
+      </c>
+      <c r="B169">
+        <v>10</v>
+      </c>
+      <c r="C169">
+        <v>4</v>
+      </c>
+      <c r="D169">
+        <v>19</v>
+      </c>
+      <c r="E169">
+        <v>41</v>
+      </c>
+      <c r="F169" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>2</v>
+      </c>
+      <c r="B170">
+        <v>10</v>
+      </c>
+      <c r="C170">
+        <v>4</v>
+      </c>
+      <c r="D170">
+        <v>29</v>
+      </c>
+      <c r="E170">
+        <v>33</v>
+      </c>
+      <c r="F170" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>2</v>
+      </c>
+      <c r="B171">
+        <v>10</v>
+      </c>
+      <c r="C171">
+        <v>4</v>
+      </c>
+      <c r="D171">
+        <v>9</v>
+      </c>
+      <c r="E171">
+        <v>43</v>
+      </c>
+      <c r="F171" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2</v>
+      </c>
+      <c r="B172">
+        <v>10</v>
+      </c>
+      <c r="C172">
+        <v>4</v>
+      </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
+      <c r="E172">
+        <v>19</v>
+      </c>
+      <c r="F172" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>2</v>
+      </c>
+      <c r="B173">
+        <v>10</v>
+      </c>
+      <c r="C173">
+        <v>4</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+      <c r="E173">
+        <v>19</v>
+      </c>
+      <c r="F173" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2</v>
+      </c>
+      <c r="B174">
+        <v>10</v>
+      </c>
+      <c r="C174">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <v>14</v>
+      </c>
+      <c r="E174">
+        <v>18</v>
+      </c>
+      <c r="F174" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>2</v>
+      </c>
+      <c r="B175">
+        <v>10</v>
+      </c>
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175">
+        <v>11</v>
+      </c>
+      <c r="E175">
+        <v>51</v>
+      </c>
+      <c r="F175" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>2</v>
+      </c>
+      <c r="B176">
+        <v>10</v>
+      </c>
+      <c r="C176">
+        <v>4</v>
+      </c>
+      <c r="D176">
+        <v>39</v>
+      </c>
+      <c r="E176">
+        <v>25</v>
+      </c>
+      <c r="F176" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2</v>
+      </c>
+      <c r="B177">
+        <v>10</v>
+      </c>
+      <c r="C177">
+        <v>4</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>52</v>
+      </c>
+      <c r="F177" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2</v>
+      </c>
+      <c r="B178">
+        <v>10</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>13</v>
+      </c>
+      <c r="F178" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>2</v>
+      </c>
+      <c r="B179">
+        <v>10</v>
+      </c>
+      <c r="C179">
+        <v>4</v>
+      </c>
+      <c r="D179">
+        <v>29</v>
+      </c>
+      <c r="E179">
+        <v>35</v>
+      </c>
+      <c r="F179" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2</v>
+      </c>
+      <c r="B180">
+        <v>10</v>
+      </c>
+      <c r="C180">
+        <v>4</v>
+      </c>
+      <c r="D180">
+        <v>13</v>
+      </c>
+      <c r="E180">
+        <v>41</v>
+      </c>
+      <c r="F180" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2</v>
+      </c>
+      <c r="B181">
+        <v>10</v>
+      </c>
+      <c r="C181">
+        <v>4</v>
+      </c>
+      <c r="D181">
+        <v>20</v>
+      </c>
+      <c r="E181">
+        <v>44</v>
+      </c>
+      <c r="F181" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>2</v>
+      </c>
+      <c r="B182">
+        <v>10</v>
+      </c>
+      <c r="C182">
+        <v>4</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>35</v>
+      </c>
+      <c r="F182" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2</v>
+      </c>
+      <c r="B183">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>4</v>
+      </c>
+      <c r="D183">
+        <v>25</v>
+      </c>
+      <c r="E183">
+        <v>38</v>
+      </c>
+      <c r="F183" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2</v>
+      </c>
+      <c r="B184">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>4</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>21</v>
+      </c>
+      <c r="F184" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2</v>
+      </c>
+      <c r="B185">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>4</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>15</v>
+      </c>
+      <c r="F185" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>2</v>
+      </c>
+      <c r="B186">
+        <v>10</v>
+      </c>
+      <c r="C186">
+        <v>4</v>
+      </c>
+      <c r="D186">
+        <v>16</v>
+      </c>
+      <c r="E186">
+        <v>46</v>
+      </c>
+      <c r="F186" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2</v>
+      </c>
+      <c r="B187">
+        <v>10</v>
+      </c>
+      <c r="C187">
+        <v>4</v>
+      </c>
+      <c r="D187">
+        <v>25</v>
+      </c>
+      <c r="E187">
+        <v>35</v>
+      </c>
+      <c r="F187" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>2</v>
+      </c>
+      <c r="B188">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <v>4</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>26</v>
+      </c>
+      <c r="F188" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2</v>
+      </c>
+      <c r="B189">
+        <v>10</v>
+      </c>
+      <c r="C189">
+        <v>4</v>
+      </c>
+      <c r="D189">
+        <v>3</v>
+      </c>
+      <c r="E189">
+        <v>56</v>
+      </c>
+      <c r="F189" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2</v>
+      </c>
+      <c r="B190">
+        <v>10</v>
+      </c>
+      <c r="C190">
+        <v>4</v>
+      </c>
+      <c r="D190">
+        <v>27</v>
+      </c>
+      <c r="E190">
+        <v>37</v>
+      </c>
+      <c r="F190" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>2</v>
+      </c>
+      <c r="B191">
+        <v>10</v>
+      </c>
+      <c r="C191">
+        <v>4</v>
+      </c>
+      <c r="D191">
+        <v>24</v>
+      </c>
+      <c r="E191">
+        <v>38</v>
+      </c>
+      <c r="F191" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>2</v>
+      </c>
+      <c r="B192">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>4</v>
+      </c>
+      <c r="D192">
+        <v>6</v>
+      </c>
+      <c r="E192">
+        <v>56</v>
+      </c>
+      <c r="F192" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>2</v>
+      </c>
+      <c r="B193">
+        <v>10</v>
+      </c>
+      <c r="C193">
+        <v>4</v>
+      </c>
+      <c r="D193">
+        <v>14</v>
+      </c>
+      <c r="E193">
+        <v>49</v>
+      </c>
+      <c r="F193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>2</v>
+      </c>
+      <c r="B194">
+        <v>10</v>
+      </c>
+      <c r="C194">
+        <v>4</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>19</v>
+      </c>
+      <c r="F194" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>2</v>
+      </c>
+      <c r="B195">
+        <v>10</v>
+      </c>
+      <c r="C195">
+        <v>4</v>
+      </c>
+      <c r="D195">
+        <v>19</v>
+      </c>
+      <c r="E195">
+        <v>45</v>
+      </c>
+      <c r="F195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>2</v>
+      </c>
+      <c r="B196">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>4</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>17</v>
+      </c>
+      <c r="F196" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>2</v>
+      </c>
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>4</v>
+      </c>
+      <c r="D197">
+        <v>41</v>
+      </c>
+      <c r="E197">
+        <v>23</v>
+      </c>
+      <c r="F197" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>2</v>
+      </c>
+      <c r="B198">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>4</v>
+      </c>
+      <c r="D198">
+        <v>18</v>
+      </c>
+      <c r="E198">
+        <v>44</v>
+      </c>
+      <c r="F198" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
+        <v>13</v>
+      </c>
+      <c r="D199">
+        <f>AVERAGE(D160:D198)</f>
+        <v>15.615384615384615</v>
+      </c>
+      <c r="E199">
+        <f>AVERAGE(E160:E198)</f>
+        <v>34.128205128205131</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C200" t="s">
+        <v>16</v>
+      </c>
+      <c r="D200">
+        <f>STDEV(D160:D198)</f>
+        <v>12.106143252640011</v>
+      </c>
+      <c r="E200">
+        <f>STDEV(E160:E198)</f>
+        <v>12.087791769035071</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>3</v>
+      </c>
+      <c r="B203">
+        <v>10</v>
+      </c>
+      <c r="C203">
+        <v>4</v>
+      </c>
+      <c r="D203">
+        <v>12</v>
+      </c>
+      <c r="E203">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>3</v>
+      </c>
+      <c r="B204">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>4</v>
+      </c>
+      <c r="D204">
+        <v>16</v>
+      </c>
+      <c r="E204">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>3</v>
+      </c>
+      <c r="B205">
+        <v>10</v>
+      </c>
+      <c r="C205">
+        <v>4</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>3</v>
+      </c>
+      <c r="B206">
+        <v>10</v>
+      </c>
+      <c r="C206">
+        <v>4</v>
+      </c>
+      <c r="D206">
+        <v>19</v>
+      </c>
+      <c r="E206">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>3</v>
+      </c>
+      <c r="B207">
+        <v>10</v>
+      </c>
+      <c r="C207">
+        <v>4</v>
+      </c>
+      <c r="D207">
+        <v>11</v>
+      </c>
+      <c r="E207">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <v>4</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+      <c r="E208">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>3</v>
+      </c>
+      <c r="B209">
+        <v>10</v>
+      </c>
+      <c r="C209">
+        <v>4</v>
+      </c>
+      <c r="D209">
+        <v>4</v>
+      </c>
+      <c r="E209">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>3</v>
+      </c>
+      <c r="B210">
+        <v>10</v>
+      </c>
+      <c r="C210">
+        <v>4</v>
+      </c>
+      <c r="D210">
+        <v>7</v>
+      </c>
+      <c r="E210">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>3</v>
+      </c>
+      <c r="B211">
+        <v>10</v>
+      </c>
+      <c r="C211">
+        <v>4</v>
+      </c>
+      <c r="D211">
+        <v>41</v>
+      </c>
+      <c r="E211">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>3</v>
+      </c>
+      <c r="B212">
+        <v>10</v>
+      </c>
+      <c r="C212">
+        <v>4</v>
+      </c>
+      <c r="D212">
+        <v>4</v>
+      </c>
+      <c r="E212">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>3</v>
+      </c>
+      <c r="B213">
+        <v>10</v>
+      </c>
+      <c r="C213">
+        <v>4</v>
+      </c>
+      <c r="D213">
+        <v>16</v>
+      </c>
+      <c r="E213">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>3</v>
+      </c>
+      <c r="B214">
+        <v>10</v>
+      </c>
+      <c r="C214">
+        <v>4</v>
+      </c>
+      <c r="D214">
+        <v>20</v>
+      </c>
+      <c r="E214">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>3</v>
+      </c>
+      <c r="B215">
+        <v>10</v>
+      </c>
+      <c r="C215">
+        <v>4</v>
+      </c>
+      <c r="D215">
+        <v>27</v>
+      </c>
+      <c r="E215">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>3</v>
+      </c>
+      <c r="B216">
+        <v>10</v>
+      </c>
+      <c r="C216">
+        <v>4</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>3</v>
+      </c>
+      <c r="B217">
+        <v>10</v>
+      </c>
+      <c r="C217">
+        <v>4</v>
+      </c>
+      <c r="D217">
+        <v>21</v>
+      </c>
+      <c r="E217">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C218" t="s">
+        <v>13</v>
+      </c>
+      <c r="D218">
+        <f>AVERAGE(D203:D217)</f>
+        <v>13.266666666666667</v>
+      </c>
+      <c r="E218">
+        <f>AVERAGE(E203:E217)</f>
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C219" t="s">
+        <v>16</v>
+      </c>
+      <c r="D219">
+        <f>STDEV(D203:D217)</f>
+        <v>11.4359499990579</v>
+      </c>
+      <c r="E219">
+        <f>STDEV(E203:E217)</f>
+        <v>12.00119041714494</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>4</v>
+      </c>
+      <c r="B222">
+        <v>10</v>
+      </c>
+      <c r="C222">
+        <v>4</v>
+      </c>
+      <c r="D222">
+        <v>19</v>
+      </c>
+      <c r="E222">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>4</v>
+      </c>
+      <c r="B223">
+        <v>10</v>
+      </c>
+      <c r="C223">
+        <v>4</v>
+      </c>
+      <c r="D223">
+        <v>19</v>
+      </c>
+      <c r="E223">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>4</v>
+      </c>
+      <c r="B224">
+        <v>10</v>
+      </c>
+      <c r="C224">
+        <v>4</v>
+      </c>
+      <c r="D224">
+        <v>33</v>
+      </c>
+      <c r="E224">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>4</v>
+      </c>
+      <c r="B225">
+        <v>10</v>
+      </c>
+      <c r="C225">
+        <v>4</v>
+      </c>
+      <c r="D225">
+        <v>5</v>
+      </c>
+      <c r="E225">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>4</v>
+      </c>
+      <c r="B226">
+        <v>10</v>
+      </c>
+      <c r="C226">
+        <v>4</v>
+      </c>
+      <c r="D226">
+        <v>27</v>
+      </c>
+      <c r="E226">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>4</v>
+      </c>
+      <c r="B227">
+        <v>10</v>
+      </c>
+      <c r="C227">
+        <v>4</v>
+      </c>
+      <c r="D227">
+        <v>30</v>
+      </c>
+      <c r="E227">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>4</v>
+      </c>
+      <c r="B228">
+        <v>10</v>
+      </c>
+      <c r="C228">
+        <v>4</v>
+      </c>
+      <c r="D228">
+        <v>18</v>
+      </c>
+      <c r="E228">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>4</v>
+      </c>
+      <c r="B229">
+        <v>10</v>
+      </c>
+      <c r="C229">
+        <v>4</v>
+      </c>
+      <c r="D229">
+        <v>22</v>
+      </c>
+      <c r="E229">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>4</v>
+      </c>
+      <c r="B230">
+        <v>10</v>
+      </c>
+      <c r="C230">
+        <v>4</v>
+      </c>
+      <c r="D230">
+        <v>22</v>
+      </c>
+      <c r="E230">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>4</v>
+      </c>
+      <c r="B231">
+        <v>10</v>
+      </c>
+      <c r="C231">
+        <v>4</v>
+      </c>
+      <c r="D231">
+        <v>22</v>
+      </c>
+      <c r="E231">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>4</v>
+      </c>
+      <c r="B232">
+        <v>10</v>
+      </c>
+      <c r="C232">
+        <v>4</v>
+      </c>
+      <c r="D232">
+        <v>18</v>
+      </c>
+      <c r="E232">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>4</v>
+      </c>
+      <c r="B233">
+        <v>10</v>
+      </c>
+      <c r="C233">
+        <v>4</v>
+      </c>
+      <c r="D233">
+        <v>28</v>
+      </c>
+      <c r="E233">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>4</v>
+      </c>
+      <c r="B234">
+        <v>10</v>
+      </c>
+      <c r="C234">
+        <v>4</v>
+      </c>
+      <c r="D234">
+        <v>7</v>
+      </c>
+      <c r="E234">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>4</v>
+      </c>
+      <c r="B235">
+        <v>10</v>
+      </c>
+      <c r="C235">
+        <v>4</v>
+      </c>
+      <c r="D235">
+        <v>43</v>
+      </c>
+      <c r="E235">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>4</v>
+      </c>
+      <c r="B236">
+        <v>10</v>
+      </c>
+      <c r="C236">
+        <v>4</v>
+      </c>
+      <c r="D236">
+        <v>5</v>
+      </c>
+      <c r="E236">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>4</v>
+      </c>
+      <c r="B237">
+        <v>10</v>
+      </c>
+      <c r="C237">
+        <v>4</v>
+      </c>
+      <c r="D237">
+        <v>28</v>
+      </c>
+      <c r="E237">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>4</v>
+      </c>
+      <c r="B238">
+        <v>10</v>
+      </c>
+      <c r="C238">
+        <v>4</v>
+      </c>
+      <c r="D238">
+        <v>32</v>
+      </c>
+      <c r="E238">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C239" t="s">
+        <v>13</v>
+      </c>
+      <c r="D239">
+        <f>AVERAGE(D222:D238)</f>
+        <v>22.235294117647058</v>
+      </c>
+      <c r="E239">
+        <f>AVERAGE(E222:E238)</f>
+        <v>37.882352941176471</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C240" t="s">
+        <v>16</v>
+      </c>
+      <c r="D240">
+        <f>STDEV(D222:D238)</f>
+        <v>10.231870624210819</v>
+      </c>
+      <c r="E240">
+        <f>STDEV(E222:E238)</f>
+        <v>9.6493675501375265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>